<commit_message>
Reto 2- Entrega final
</commit_message>
<xml_diff>
--- a/Docs/Pruebas .xlsx
+++ b/Docs/Pruebas .xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1902876135bf28ab/Documents/EDA/Reto 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\vs repositorios\Reto2-G04\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{78D16272-9CB3-49EF-AA6E-D8B610964452}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{93EA112B-511F-4F0D-B1DC-DD6FE917A542}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F3B5E6-B7EF-494A-A56F-B9F2401AA0BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{68679276-25EC-4906-9412-406552415E59}"/>
+    <workbookView xWindow="26820" yWindow="7935" windowWidth="2400" windowHeight="585" xr2:uid="{68679276-25EC-4906-9412-406552415E59}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -82,8 +73,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -135,11 +127,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,19 +450,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F69E4E3-20DF-4467-AAC8-6AED35395C97}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -503,37 +498,77 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="B2" s="3">
+        <v>948.76800000000003</v>
+      </c>
+      <c r="C2" s="1">
+        <v>306.76499999999999</v>
+      </c>
+      <c r="D2" s="5">
+        <v>1010695.5</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2210.2260000000001</v>
+      </c>
+      <c r="F2" s="4">
+        <v>312864.71799999999</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1142.0319999999999</v>
+      </c>
+      <c r="H2" s="3">
+        <v>615.78700000000003</v>
+      </c>
+      <c r="I2" s="3">
+        <v>630.02700000000004</v>
+      </c>
+      <c r="J2" s="3">
+        <v>63490.591999999997</v>
+      </c>
+      <c r="K2" s="1">
+        <v>128236.251</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="B3" s="3">
+        <v>36.027000000000001</v>
+      </c>
+      <c r="C3" s="3">
+        <v>40.729999999999997</v>
+      </c>
+      <c r="D3" s="1">
+        <v>18046.993999999999</v>
+      </c>
+      <c r="E3" s="4">
+        <v>200090</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3926.3629999999998</v>
+      </c>
+      <c r="G3" s="5">
+        <v>86.98</v>
+      </c>
+      <c r="H3" s="3">
+        <v>50.097999999999999</v>
+      </c>
+      <c r="I3" s="3">
+        <v>49.551000000000002</v>
+      </c>
+      <c r="J3" s="4">
+        <v>1647366.5689999999</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1882234.9210000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -568,7 +603,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -603,7 +638,7 @@
         <v>58491.196000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>